<commit_message>
task 5 in progress
</commit_message>
<xml_diff>
--- a/Статистика.xlsx
+++ b/Статистика.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Technopark\semester_3\highload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ACE119-165E-45AC-8753-42457F73C919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24E15BB-ABFE-456A-BA0E-EEDE3B97B6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Имя пользователя</t>
   </si>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AK17" sqref="AK17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,14 +603,17 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>15800</v>
+        <v>1900</v>
       </c>
       <c r="I2" s="1">
-        <v>821</v>
+        <v>41</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -676,11 +679,14 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
       <c r="G3" s="1">
         <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -749,14 +755,17 @@
       <c r="D4" s="1">
         <v>65</v>
       </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
       <c r="G4" s="1">
         <v>3</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1">
         <v>3</v>
@@ -822,14 +831,17 @@
       <c r="D5" s="1">
         <v>164</v>
       </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
       <c r="G5" s="1">
         <v>4</v>
       </c>
       <c r="H5" s="1">
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>509</v>
+        <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
@@ -895,11 +907,14 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
       <c r="G6" s="1">
         <v>5</v>
       </c>
       <c r="H6" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -968,14 +983,17 @@
       <c r="D7" s="1">
         <v>50</v>
       </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
       <c r="G7" s="1">
         <v>6</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>634</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="L7" s="1">
         <v>6</v>
@@ -1041,14 +1059,17 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
       <c r="G8" s="1">
         <v>7</v>
       </c>
       <c r="H8" s="1">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="I8" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="L8" s="1">
         <v>7</v>
@@ -1114,14 +1135,17 @@
       <c r="D9" s="1">
         <v>451</v>
       </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
       <c r="G9" s="1">
         <v>8</v>
       </c>
       <c r="H9" s="1">
-        <v>198</v>
+        <v>2600</v>
       </c>
       <c r="I9" s="1">
-        <v>26</v>
+        <v>401</v>
       </c>
       <c r="L9" s="1">
         <v>8</v>
@@ -1187,14 +1211,17 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
       <c r="G10" s="1">
         <v>9</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L10" s="1">
         <v>9</v>
@@ -1260,14 +1287,17 @@
       <c r="D11" s="1">
         <v>928</v>
       </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
       <c r="G11" s="1">
         <v>10</v>
       </c>
       <c r="H11" s="1">
-        <v>6200</v>
+        <v>130</v>
       </c>
       <c r="I11" s="1">
-        <v>183</v>
+        <v>3</v>
       </c>
       <c r="L11" s="1">
         <v>10</v>
@@ -1333,14 +1363,17 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
       <c r="G12" s="1">
         <v>11</v>
       </c>
       <c r="H12" s="1">
-        <v>15300</v>
+        <v>619</v>
       </c>
       <c r="I12" s="1">
-        <v>1400</v>
+        <v>23</v>
       </c>
       <c r="L12" s="1">
         <v>11</v>
@@ -1412,14 +1445,17 @@
       <c r="D13" s="1">
         <v>275</v>
       </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
       <c r="G13" s="1">
         <v>12</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L13" s="1">
         <v>12</v>
@@ -1491,14 +1527,17 @@
       <c r="D14" s="1">
         <v>420</v>
       </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
       <c r="G14" s="1">
         <v>13</v>
       </c>
       <c r="H14" s="1">
-        <v>2400</v>
+        <v>8</v>
       </c>
       <c r="I14" s="1">
-        <v>197</v>
+        <v>2</v>
       </c>
       <c r="L14" s="1">
         <v>13</v>
@@ -1535,11 +1574,14 @@
       <c r="D15" s="1">
         <v>207</v>
       </c>
+      <c r="E15" s="1">
+        <v>14</v>
+      </c>
       <c r="G15" s="1">
         <v>14</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -1579,14 +1621,17 @@
       <c r="D16" s="1">
         <v>435</v>
       </c>
+      <c r="E16" s="1">
+        <v>15</v>
+      </c>
       <c r="G16" s="1">
         <v>15</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>7800</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>435</v>
       </c>
       <c r="L16" s="1">
         <v>15</v>
@@ -1623,14 +1668,17 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
       <c r="G17" s="1">
         <v>16</v>
       </c>
       <c r="H17" s="1">
-        <v>2400</v>
+        <v>12</v>
       </c>
       <c r="I17" s="1">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="L17" s="1">
         <v>16</v>
@@ -1667,14 +1715,17 @@
       <c r="D18" s="1">
         <v>4</v>
       </c>
+      <c r="E18" s="1">
+        <v>17</v>
+      </c>
       <c r="G18" s="1">
         <v>17</v>
       </c>
       <c r="H18" s="1">
-        <v>1500</v>
+        <v>405</v>
       </c>
       <c r="I18" s="1">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="L18" s="1">
         <v>17</v>
@@ -1711,14 +1762,17 @@
       <c r="D19" s="1">
         <v>55</v>
       </c>
+      <c r="E19" s="1">
+        <v>18</v>
+      </c>
       <c r="G19" s="1">
         <v>18</v>
       </c>
       <c r="H19" s="1">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L19" s="1">
         <v>18</v>
@@ -1755,14 +1809,17 @@
       <c r="D20" s="1">
         <v>13</v>
       </c>
+      <c r="E20" s="1">
+        <v>19</v>
+      </c>
       <c r="G20" s="1">
         <v>19</v>
       </c>
       <c r="H20" s="1">
-        <v>1100</v>
+        <v>760</v>
       </c>
       <c r="I20" s="1">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="L20" s="1">
         <v>19</v>
@@ -1799,14 +1856,17 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
       <c r="G21" s="1">
         <v>20</v>
       </c>
       <c r="H21" s="1">
-        <v>16</v>
+        <v>8400</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>297</v>
       </c>
       <c r="L21" s="1">
         <v>20</v>
@@ -1843,14 +1903,17 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
+      <c r="E22" s="1">
+        <v>21</v>
+      </c>
       <c r="G22" s="1">
         <v>21</v>
       </c>
       <c r="H22" s="1">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="1">
         <v>21</v>
@@ -1887,14 +1950,17 @@
       <c r="D23" s="1">
         <v>16</v>
       </c>
+      <c r="E23" s="1">
+        <v>22</v>
+      </c>
       <c r="G23" s="1">
         <v>22</v>
       </c>
       <c r="H23" s="1">
-        <v>866</v>
+        <v>53</v>
       </c>
       <c r="I23" s="1">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="L23" s="1">
         <v>22</v>
@@ -1931,14 +1997,17 @@
       <c r="D24" s="1">
         <v>7</v>
       </c>
+      <c r="E24" s="1">
+        <v>23</v>
+      </c>
       <c r="G24" s="1">
         <v>23</v>
       </c>
       <c r="H24" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
         <v>23</v>
@@ -1975,11 +2044,14 @@
       <c r="D25" s="1">
         <v>48</v>
       </c>
+      <c r="E25" s="1">
+        <v>24</v>
+      </c>
       <c r="G25" s="1">
         <v>24</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -2019,14 +2091,17 @@
       <c r="D26" s="1">
         <v>11</v>
       </c>
+      <c r="E26" s="1">
+        <v>25</v>
+      </c>
       <c r="G26" s="1">
         <v>25</v>
       </c>
       <c r="H26" s="1">
-        <v>6700</v>
+        <v>6800</v>
       </c>
       <c r="I26" s="1">
-        <v>698</v>
+        <v>363</v>
       </c>
       <c r="L26" s="1">
         <v>25</v>
@@ -2063,14 +2138,17 @@
       <c r="D27" s="1">
         <v>13</v>
       </c>
+      <c r="E27" s="1">
+        <v>26</v>
+      </c>
       <c r="G27" s="1">
         <v>26</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27" s="1">
         <v>26</v>
@@ -2114,10 +2192,10 @@
         <v>27</v>
       </c>
       <c r="H28" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I28" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L28" s="1">
         <v>27</v>
@@ -2142,18 +2220,29 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <f>B28/$E$27</f>
+        <v>1413.2692307692307</v>
+      </c>
+      <c r="C29" s="1">
+        <f>C28/$E$27</f>
+        <v>108.5</v>
+      </c>
+      <c r="D29" s="1">
+        <f>D28/$E$27</f>
+        <v>121.96153846153847</v>
+      </c>
       <c r="G29" s="1">
         <v>28</v>
       </c>
       <c r="H29" s="1">
-        <v>2</v>
+        <v>2500</v>
       </c>
       <c r="I29" s="1">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="L29" s="1">
         <v>28</v>
@@ -2186,10 +2275,10 @@
         <v>29</v>
       </c>
       <c r="H30" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30" s="1">
         <v>29</v>
@@ -2218,7 +2307,7 @@
         <v>30</v>
       </c>
       <c r="H31" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -2251,11 +2340,11 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" ref="H32:I32" si="1">SUM(H2:H31)</f>
-        <v>54689</v>
+        <v>34124</v>
       </c>
       <c r="I32" s="1">
         <f t="shared" si="1"/>
-        <v>4263</v>
+        <v>1860</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>30</v>
@@ -2287,11 +2376,11 @@
       </c>
       <c r="H33" s="1">
         <f>H32/G31</f>
-        <v>1822.9666666666667</v>
+        <v>1137.4666666666667</v>
       </c>
       <c r="I33" s="1">
         <f>I32/G31</f>
-        <v>142.1</v>
+        <v>62</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>34</v>

</xml_diff>